<commit_message>
Added compiling tools via pyinstaller
</commit_message>
<xml_diff>
--- a/test_template_filled.xlsx
+++ b/test_template_filled.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\galizia_lab_equipment\galizia-lab-equipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\galizia-lab-equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B460360-EEE5-4758-AA05-8AE6FBE57368}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDB0DE1-37C2-44B6-8373-7FAE087976E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24990" yWindow="3450" windowWidth="7500" windowHeight="9390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>temperature</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>final pressure of the charge chamber after valve close</t>
+  </si>
+  <si>
+    <t>afgsdfgdsfg</t>
   </si>
 </sst>
 </file>
@@ -479,15 +482,15 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -607,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -700,7 +703,7 @@
         <v>7025.7078947399996</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>6</v>
       </c>
@@ -710,8 +713,11 @@
       <c r="C17" s="1">
         <v>8417.0855263199992</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="C18" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrapped up vapor tests
</commit_message>
<xml_diff>
--- a/test_template_filled.xlsx
+++ b/test_template_filled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\galizia-lab-equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDB0DE1-37C2-44B6-8373-7FAE087976E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50397FC-947D-49B4-9FDA-3F5F86900B44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30540" yWindow="4515" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -610,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>10000000</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>

</xml_diff>